<commit_message>
Update consumer insights dashboard
</commit_message>
<xml_diff>
--- a/Untitled spreadsheet.xlsx
+++ b/Untitled spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/advikholalu/Desktop/insightsgraphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B36B87-63C3-E349-BC5F-92AD88050519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4547B05-278C-524C-A86C-1875DA6C3331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -2599,7 +2599,7 @@
   </sheetPr>
   <dimension ref="A1:AB999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -44096,8 +44096,8 @@
   </sheetPr>
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="G9" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Update Jan 3rd week,  dynamic percentages, no row drops
</commit_message>
<xml_diff>
--- a/Untitled spreadsheet.xlsx
+++ b/Untitled spreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/advikholalu/Desktop/insightsgraphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16E50BE-B8DC-5740-9A61-3CDCE780FD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806D13F0-3BD1-4B45-95ED-2C11A83CE7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sweets" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$1:$P$428</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$1:$P$468</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8308" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8794" uniqueCount="1011">
   <si>
     <t>Customer Name</t>
   </si>
@@ -2951,6 +2951,126 @@
   </si>
   <si>
     <t>Daadi</t>
+  </si>
+  <si>
+    <t>Murali Shankar Reddy</t>
+  </si>
+  <si>
+    <t>Tanmay Raut</t>
+  </si>
+  <si>
+    <t>Bhumi Hada</t>
+  </si>
+  <si>
+    <t>Deepthi shree</t>
+  </si>
+  <si>
+    <t>Sofia Taneja</t>
+  </si>
+  <si>
+    <t>Vineeta Vineeta</t>
+  </si>
+  <si>
+    <t>Amit kumar satapathy</t>
+  </si>
+  <si>
+    <t>DINESH KUMAR</t>
+  </si>
+  <si>
+    <t>Bhagyashree nanda</t>
+  </si>
+  <si>
+    <t>Washim Akram</t>
+  </si>
+  <si>
+    <t>Anita meena</t>
+  </si>
+  <si>
+    <t>Rajesh kumar kothuri</t>
+  </si>
+  <si>
+    <t>She dont prefer sweets anymore</t>
+  </si>
+  <si>
+    <t>Disconnected the call</t>
+  </si>
+  <si>
+    <t>Bikanervala, Haldiram's, Prefers whatever's convenient</t>
+  </si>
+  <si>
+    <t>Amul, Haldiram's, GODESi</t>
+  </si>
+  <si>
+    <t>Amul, Farmley, Yogabar</t>
+  </si>
+  <si>
+    <t>Jinosha jose</t>
+  </si>
+  <si>
+    <t>Nimisha Kankan</t>
+  </si>
+  <si>
+    <t>Ganesh</t>
+  </si>
+  <si>
+    <t>mithun Bg</t>
+  </si>
+  <si>
+    <t>suraj</t>
+  </si>
+  <si>
+    <t>Niraj chand</t>
+  </si>
+  <si>
+    <t>Pooja</t>
+  </si>
+  <si>
+    <t>Revathi </t>
+  </si>
+  <si>
+    <t>Jagriti Choudhary</t>
+  </si>
+  <si>
+    <t>Shruthika nair</t>
+  </si>
+  <si>
+    <t>Kusum lata</t>
+  </si>
+  <si>
+    <t>Madhuri jadhav</t>
+  </si>
+  <si>
+    <t>Vinay TS</t>
+  </si>
+  <si>
+    <t>Keith Michael</t>
+  </si>
+  <si>
+    <t>Karina parvin</t>
+  </si>
+  <si>
+    <t>Taher hussain</t>
+  </si>
+  <si>
+    <t>Justeen koola</t>
+  </si>
+  <si>
+    <t>google </t>
+  </si>
+  <si>
+    <t>In the evening</t>
+  </si>
+  <si>
+    <t>Better Ingredients, Since he is a reseller of our products and they are fast-moving</t>
+  </si>
+  <si>
+    <t>Chapati cravings, Better Ingredients, Guilt free snacking</t>
+  </si>
+  <si>
+    <t>Better Ingredients, Nostalgic vibes, Guilt free snacking</t>
+  </si>
+  <si>
+    <t>He ordered it for his kids</t>
   </si>
 </sst>
 </file>
@@ -3274,10 +3394,10 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D424" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D464" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I419" sqref="I419"/>
+      <selection pane="bottomRight" activeCell="G475" sqref="G475"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30489,22 +30609,54 @@
       <c r="Z455" s="2"/>
     </row>
     <row r="456" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A456" s="2"/>
-      <c r="B456" s="2"/>
-      <c r="C456" s="2"/>
-      <c r="D456" s="2"/>
-      <c r="E456" s="2"/>
-      <c r="F456" s="2"/>
-      <c r="G456" s="2"/>
-      <c r="H456" s="2"/>
-      <c r="I456" s="2"/>
-      <c r="J456" s="2"/>
-      <c r="K456" s="2"/>
-      <c r="L456" s="2"/>
-      <c r="M456" s="2"/>
-      <c r="N456" s="2"/>
-      <c r="O456" s="2"/>
-      <c r="P456" s="2"/>
+      <c r="A456" s="5" t="s">
+        <v>971</v>
+      </c>
+      <c r="B456" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C456" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D456" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E456" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F456" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G456" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H456" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I456" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J456" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K456" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L456" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="M456" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="N456" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O456" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="P456" s="5" t="s">
+        <v>260</v>
+      </c>
       <c r="Q456" s="2"/>
       <c r="R456" s="2"/>
       <c r="S456" s="2"/>
@@ -30517,22 +30669,54 @@
       <c r="Z456" s="2"/>
     </row>
     <row r="457" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A457" s="2"/>
-      <c r="B457" s="2"/>
-      <c r="C457" s="2"/>
-      <c r="D457" s="2"/>
-      <c r="E457" s="2"/>
-      <c r="F457" s="2"/>
-      <c r="G457" s="2"/>
-      <c r="H457" s="2"/>
-      <c r="I457" s="2"/>
-      <c r="J457" s="2"/>
-      <c r="K457" s="2"/>
-      <c r="L457" s="2"/>
-      <c r="M457" s="2"/>
-      <c r="N457" s="2"/>
-      <c r="O457" s="2"/>
-      <c r="P457" s="2"/>
+      <c r="A457" s="5" t="s">
+        <v>972</v>
+      </c>
+      <c r="B457" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C457" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D457" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E457" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F457" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G457" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H457" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I457" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J457" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K457" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L457" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="M457" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="N457" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="O457" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="P457" s="5" t="s">
+        <v>262</v>
+      </c>
       <c r="Q457" s="2"/>
       <c r="R457" s="2"/>
       <c r="S457" s="2"/>
@@ -30545,22 +30729,54 @@
       <c r="Z457" s="2"/>
     </row>
     <row r="458" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A458" s="2"/>
-      <c r="B458" s="2"/>
-      <c r="C458" s="2"/>
-      <c r="D458" s="2"/>
-      <c r="E458" s="2"/>
-      <c r="F458" s="2"/>
-      <c r="G458" s="2"/>
-      <c r="H458" s="2"/>
-      <c r="I458" s="2"/>
-      <c r="J458" s="2"/>
-      <c r="K458" s="2"/>
-      <c r="L458" s="2"/>
-      <c r="M458" s="2"/>
-      <c r="N458" s="2"/>
-      <c r="O458" s="2"/>
-      <c r="P458" s="2"/>
+      <c r="A458" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B458" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C458" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D458" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E458" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F458" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G458" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H458" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I458" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J458" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K458" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L458" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="M458" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="N458" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="O458" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="P458" s="5" t="s">
+        <v>262</v>
+      </c>
       <c r="Q458" s="2"/>
       <c r="R458" s="2"/>
       <c r="S458" s="2"/>
@@ -30573,22 +30789,54 @@
       <c r="Z458" s="2"/>
     </row>
     <row r="459" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A459" s="2"/>
-      <c r="B459" s="2"/>
-      <c r="C459" s="2"/>
-      <c r="D459" s="2"/>
-      <c r="E459" s="2"/>
-      <c r="F459" s="2"/>
-      <c r="G459" s="2"/>
-      <c r="H459" s="2"/>
-      <c r="I459" s="2"/>
-      <c r="J459" s="2"/>
-      <c r="K459" s="2"/>
-      <c r="L459" s="2"/>
-      <c r="M459" s="2"/>
-      <c r="N459" s="2"/>
-      <c r="O459" s="2"/>
-      <c r="P459" s="2"/>
+      <c r="A459" s="5" t="s">
+        <v>974</v>
+      </c>
+      <c r="B459" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C459" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D459" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E459" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F459" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G459" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H459" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I459" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J459" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K459" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L459" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="M459" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="N459" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="O459" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="P459" s="5" t="s">
+        <v>266</v>
+      </c>
       <c r="Q459" s="2"/>
       <c r="R459" s="2"/>
       <c r="S459" s="2"/>
@@ -30601,22 +30849,54 @@
       <c r="Z459" s="2"/>
     </row>
     <row r="460" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A460" s="2"/>
-      <c r="B460" s="2"/>
-      <c r="C460" s="2"/>
-      <c r="D460" s="2"/>
-      <c r="E460" s="2"/>
-      <c r="F460" s="2"/>
-      <c r="G460" s="2"/>
-      <c r="H460" s="2"/>
-      <c r="I460" s="2"/>
-      <c r="J460" s="2"/>
-      <c r="K460" s="2"/>
-      <c r="L460" s="2"/>
-      <c r="M460" s="2"/>
-      <c r="N460" s="2"/>
-      <c r="O460" s="2"/>
-      <c r="P460" s="2"/>
+      <c r="A460" s="5" t="s">
+        <v>975</v>
+      </c>
+      <c r="B460" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C460" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D460" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E460" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F460" s="5" t="s">
+        <v>952</v>
+      </c>
+      <c r="G460" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H460" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I460" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J460" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K460" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L460" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="M460" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="N460" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="O460" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="P460" s="5" t="s">
+        <v>983</v>
+      </c>
       <c r="Q460" s="2"/>
       <c r="R460" s="2"/>
       <c r="S460" s="2"/>
@@ -30629,22 +30909,54 @@
       <c r="Z460" s="2"/>
     </row>
     <row r="461" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A461" s="2"/>
-      <c r="B461" s="2"/>
-      <c r="C461" s="2"/>
-      <c r="D461" s="2"/>
-      <c r="E461" s="2"/>
-      <c r="F461" s="2"/>
-      <c r="G461" s="2"/>
-      <c r="H461" s="2"/>
-      <c r="I461" s="2"/>
-      <c r="J461" s="2"/>
-      <c r="K461" s="2"/>
-      <c r="L461" s="2"/>
-      <c r="M461" s="2"/>
-      <c r="N461" s="2"/>
-      <c r="O461" s="2"/>
-      <c r="P461" s="2"/>
+      <c r="A461" s="5" t="s">
+        <v>976</v>
+      </c>
+      <c r="B461" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C461" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D461" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E461" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F461" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G461" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H461" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I461" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J461" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K461" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L461" s="5" t="s">
+        <v>984</v>
+      </c>
+      <c r="M461" s="5" t="s">
+        <v>984</v>
+      </c>
+      <c r="N461" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="O461" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="P461" s="5" t="s">
+        <v>265</v>
+      </c>
       <c r="Q461" s="2"/>
       <c r="R461" s="2"/>
       <c r="S461" s="2"/>
@@ -30657,22 +30969,54 @@
       <c r="Z461" s="2"/>
     </row>
     <row r="462" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A462" s="2"/>
-      <c r="B462" s="2"/>
-      <c r="C462" s="2"/>
-      <c r="D462" s="2"/>
-      <c r="E462" s="2"/>
-      <c r="F462" s="2"/>
-      <c r="G462" s="2"/>
-      <c r="H462" s="2"/>
-      <c r="I462" s="2"/>
-      <c r="J462" s="2"/>
-      <c r="K462" s="2"/>
-      <c r="L462" s="2"/>
-      <c r="M462" s="2"/>
-      <c r="N462" s="2"/>
-      <c r="O462" s="2"/>
-      <c r="P462" s="2"/>
+      <c r="A462" s="5" t="s">
+        <v>977</v>
+      </c>
+      <c r="B462" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C462" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D462" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E462" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F462" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G462" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H462" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I462" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J462" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K462" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L462" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="M462" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="N462" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O462" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="P462" s="5" t="s">
+        <v>262</v>
+      </c>
       <c r="Q462" s="2"/>
       <c r="R462" s="2"/>
       <c r="S462" s="2"/>
@@ -30685,22 +31029,54 @@
       <c r="Z462" s="2"/>
     </row>
     <row r="463" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A463" s="2"/>
-      <c r="B463" s="2"/>
-      <c r="C463" s="2"/>
-      <c r="D463" s="2"/>
-      <c r="E463" s="2"/>
-      <c r="F463" s="2"/>
-      <c r="G463" s="2"/>
-      <c r="H463" s="2"/>
-      <c r="I463" s="2"/>
-      <c r="J463" s="2"/>
-      <c r="K463" s="2"/>
-      <c r="L463" s="2"/>
-      <c r="M463" s="2"/>
-      <c r="N463" s="2"/>
-      <c r="O463" s="2"/>
-      <c r="P463" s="2"/>
+      <c r="A463" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B463" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C463" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D463" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E463" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F463" s="5" t="s">
+        <v>952</v>
+      </c>
+      <c r="G463" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H463" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I463" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J463" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K463" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L463" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="M463" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="N463" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="O463" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="P463" s="5" t="s">
+        <v>265</v>
+      </c>
       <c r="Q463" s="2"/>
       <c r="R463" s="2"/>
       <c r="S463" s="2"/>
@@ -30713,22 +31089,54 @@
       <c r="Z463" s="2"/>
     </row>
     <row r="464" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A464" s="2"/>
-      <c r="B464" s="2"/>
-      <c r="C464" s="2"/>
-      <c r="D464" s="2"/>
-      <c r="E464" s="2"/>
-      <c r="F464" s="2"/>
-      <c r="G464" s="2"/>
-      <c r="H464" s="2"/>
-      <c r="I464" s="2"/>
-      <c r="J464" s="2"/>
-      <c r="K464" s="2"/>
-      <c r="L464" s="2"/>
-      <c r="M464" s="2"/>
-      <c r="N464" s="2"/>
-      <c r="O464" s="2"/>
-      <c r="P464" s="2"/>
+      <c r="A464" s="5" t="s">
+        <v>979</v>
+      </c>
+      <c r="B464" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C464" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D464" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E464" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F464" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G464" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H464" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I464" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J464" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K464" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L464" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="M464" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="N464" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="O464" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="P464" s="5" t="s">
+        <v>262</v>
+      </c>
       <c r="Q464" s="2"/>
       <c r="R464" s="2"/>
       <c r="S464" s="2"/>
@@ -30741,22 +31149,54 @@
       <c r="Z464" s="2"/>
     </row>
     <row r="465" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A465" s="2"/>
-      <c r="B465" s="2"/>
-      <c r="C465" s="2"/>
-      <c r="D465" s="2"/>
-      <c r="E465" s="2"/>
-      <c r="F465" s="2"/>
-      <c r="G465" s="2"/>
-      <c r="H465" s="2"/>
-      <c r="I465" s="2"/>
-      <c r="J465" s="2"/>
-      <c r="K465" s="2"/>
-      <c r="L465" s="2"/>
-      <c r="M465" s="2"/>
-      <c r="N465" s="2"/>
-      <c r="O465" s="2"/>
-      <c r="P465" s="2"/>
+      <c r="A465" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="B465" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C465" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D465" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E465" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F465" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G465" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H465" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I465" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J465" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K465" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L465" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="M465" s="5" t="s">
+        <v>986</v>
+      </c>
+      <c r="N465" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="O465" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="P465" s="5" t="s">
+        <v>267</v>
+      </c>
       <c r="Q465" s="2"/>
       <c r="R465" s="2"/>
       <c r="S465" s="2"/>
@@ -30769,22 +31209,54 @@
       <c r="Z465" s="2"/>
     </row>
     <row r="466" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A466" s="2"/>
-      <c r="B466" s="2"/>
-      <c r="C466" s="2"/>
-      <c r="D466" s="2"/>
-      <c r="E466" s="2"/>
-      <c r="F466" s="2"/>
-      <c r="G466" s="2"/>
-      <c r="H466" s="2"/>
-      <c r="I466" s="2"/>
-      <c r="J466" s="2"/>
-      <c r="K466" s="2"/>
-      <c r="L466" s="2"/>
-      <c r="M466" s="2"/>
-      <c r="N466" s="2"/>
-      <c r="O466" s="2"/>
-      <c r="P466" s="2"/>
+      <c r="A466" s="5" t="s">
+        <v>980</v>
+      </c>
+      <c r="B466" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C466" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D466" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E466" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F466" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G466" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H466" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I466" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J466" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K466" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L466" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="M466" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="N466" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="O466" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="P466" s="5" t="s">
+        <v>266</v>
+      </c>
       <c r="Q466" s="2"/>
       <c r="R466" s="2"/>
       <c r="S466" s="2"/>
@@ -30797,22 +31269,54 @@
       <c r="Z466" s="2"/>
     </row>
     <row r="467" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A467" s="2"/>
-      <c r="B467" s="2"/>
-      <c r="C467" s="2"/>
-      <c r="D467" s="2"/>
-      <c r="E467" s="2"/>
-      <c r="F467" s="2"/>
-      <c r="G467" s="2"/>
-      <c r="H467" s="2"/>
-      <c r="I467" s="2"/>
-      <c r="J467" s="2"/>
-      <c r="K467" s="2"/>
-      <c r="L467" s="2"/>
-      <c r="M467" s="2"/>
-      <c r="N467" s="2"/>
-      <c r="O467" s="2"/>
-      <c r="P467" s="2"/>
+      <c r="A467" s="5" t="s">
+        <v>981</v>
+      </c>
+      <c r="B467" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C467" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D467" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E467" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F467" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G467" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H467" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I467" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J467" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K467" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L467" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="M467" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="N467" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="O467" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="P467" s="5" t="s">
+        <v>266</v>
+      </c>
       <c r="Q467" s="2"/>
       <c r="R467" s="2"/>
       <c r="S467" s="2"/>
@@ -30825,22 +31329,54 @@
       <c r="Z467" s="2"/>
     </row>
     <row r="468" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A468" s="2"/>
-      <c r="B468" s="2"/>
-      <c r="C468" s="2"/>
-      <c r="D468" s="2"/>
-      <c r="E468" s="2"/>
-      <c r="F468" s="2"/>
-      <c r="G468" s="2"/>
-      <c r="H468" s="2"/>
-      <c r="I468" s="2"/>
-      <c r="J468" s="2"/>
-      <c r="K468" s="2"/>
-      <c r="L468" s="2"/>
-      <c r="M468" s="2"/>
-      <c r="N468" s="2"/>
-      <c r="O468" s="2"/>
-      <c r="P468" s="2"/>
+      <c r="A468" s="5" t="s">
+        <v>982</v>
+      </c>
+      <c r="B468" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C468" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D468" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E468" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F468" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="G468" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H468" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I468" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J468" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K468" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L468" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="M468" s="5" t="s">
+        <v>987</v>
+      </c>
+      <c r="N468" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O468" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="P468" s="5" t="s">
+        <v>474</v>
+      </c>
       <c r="Q468" s="2"/>
       <c r="R468" s="2"/>
       <c r="S468" s="2"/>
@@ -30853,22 +31389,54 @@
       <c r="Z468" s="2"/>
     </row>
     <row r="469" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A469" s="2"/>
-      <c r="B469" s="2"/>
-      <c r="C469" s="2"/>
-      <c r="D469" s="2"/>
-      <c r="E469" s="2"/>
-      <c r="F469" s="2"/>
-      <c r="G469" s="2"/>
-      <c r="H469" s="2"/>
-      <c r="I469" s="2"/>
-      <c r="J469" s="2"/>
-      <c r="K469" s="2"/>
-      <c r="L469" s="2"/>
-      <c r="M469" s="2"/>
-      <c r="N469" s="2"/>
-      <c r="O469" s="2"/>
-      <c r="P469" s="2"/>
+      <c r="A469" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B469" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C469" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D469" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E469" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F469" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G469" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H469" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="I469" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="J469" s="5" t="s">
+        <v>918</v>
+      </c>
+      <c r="K469" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L469" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M469" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N469" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O469" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P469" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q469" s="2"/>
       <c r="R469" s="2"/>
       <c r="S469" s="2"/>
@@ -30881,22 +31449,54 @@
       <c r="Z469" s="2"/>
     </row>
     <row r="470" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A470" s="2"/>
-      <c r="B470" s="2"/>
-      <c r="C470" s="2"/>
-      <c r="D470" s="2"/>
-      <c r="E470" s="2"/>
-      <c r="F470" s="2"/>
-      <c r="G470" s="2"/>
-      <c r="H470" s="2"/>
-      <c r="I470" s="2"/>
-      <c r="J470" s="2"/>
-      <c r="K470" s="2"/>
-      <c r="L470" s="2"/>
-      <c r="M470" s="2"/>
-      <c r="N470" s="2"/>
-      <c r="O470" s="2"/>
-      <c r="P470" s="2"/>
+      <c r="A470" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="B470" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C470" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D470" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E470" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F470" s="5" t="s">
+        <v>1005</v>
+      </c>
+      <c r="G470" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H470" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="I470" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J470" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="K470" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L470" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M470" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N470" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O470" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P470" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q470" s="2"/>
       <c r="R470" s="2"/>
       <c r="S470" s="2"/>
@@ -30909,22 +31509,48 @@
       <c r="Z470" s="2"/>
     </row>
     <row r="471" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A471" s="2"/>
-      <c r="B471" s="2"/>
-      <c r="C471" s="2"/>
-      <c r="D471" s="2"/>
-      <c r="E471" s="2"/>
-      <c r="F471" s="2"/>
-      <c r="G471" s="2"/>
-      <c r="H471" s="2"/>
-      <c r="I471" s="2"/>
-      <c r="J471" s="2"/>
-      <c r="K471" s="2"/>
-      <c r="L471" s="2"/>
-      <c r="M471" s="2"/>
-      <c r="N471" s="2"/>
-      <c r="O471" s="2"/>
-      <c r="P471" s="2"/>
+      <c r="A471" s="5" t="s">
+        <v>990</v>
+      </c>
+      <c r="B471" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C471" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D471" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E471" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F471" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G471" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H471" s="6"/>
+      <c r="I471" s="6"/>
+      <c r="J471" s="6"/>
+      <c r="K471" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L471" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M471" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N471" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O471" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P471" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q471" s="2"/>
       <c r="R471" s="2"/>
       <c r="S471" s="2"/>
@@ -30937,22 +31563,54 @@
       <c r="Z471" s="2"/>
     </row>
     <row r="472" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A472" s="2"/>
-      <c r="B472" s="2"/>
-      <c r="C472" s="2"/>
-      <c r="D472" s="2"/>
-      <c r="E472" s="2"/>
-      <c r="F472" s="2"/>
-      <c r="G472" s="2"/>
-      <c r="H472" s="2"/>
-      <c r="I472" s="2"/>
-      <c r="J472" s="2"/>
-      <c r="K472" s="2"/>
-      <c r="L472" s="2"/>
-      <c r="M472" s="2"/>
-      <c r="N472" s="2"/>
-      <c r="O472" s="2"/>
-      <c r="P472" s="2"/>
+      <c r="A472" s="5" t="s">
+        <v>991</v>
+      </c>
+      <c r="B472" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C472" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D472" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E472" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F472" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G472" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H472" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="I472" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="J472" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="K472" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L472" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M472" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N472" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O472" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P472" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q472" s="2"/>
       <c r="R472" s="2"/>
       <c r="S472" s="2"/>
@@ -30965,22 +31623,54 @@
       <c r="Z472" s="2"/>
     </row>
     <row r="473" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A473" s="2"/>
-      <c r="B473" s="2"/>
-      <c r="C473" s="2"/>
-      <c r="D473" s="2"/>
-      <c r="E473" s="2"/>
-      <c r="F473" s="2"/>
-      <c r="G473" s="2"/>
-      <c r="H473" s="2"/>
-      <c r="I473" s="2"/>
-      <c r="J473" s="2"/>
-      <c r="K473" s="2"/>
-      <c r="L473" s="2"/>
-      <c r="M473" s="2"/>
-      <c r="N473" s="2"/>
-      <c r="O473" s="2"/>
-      <c r="P473" s="2"/>
+      <c r="A473" s="5" t="s">
+        <v>992</v>
+      </c>
+      <c r="B473" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C473" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D473" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E473" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F473" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G473" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H473" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="I473" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="J473" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="K473" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L473" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M473" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N473" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O473" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P473" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q473" s="2"/>
       <c r="R473" s="2"/>
       <c r="S473" s="2"/>
@@ -30993,22 +31683,54 @@
       <c r="Z473" s="2"/>
     </row>
     <row r="474" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A474" s="2"/>
-      <c r="B474" s="2"/>
-      <c r="C474" s="2"/>
-      <c r="D474" s="2"/>
-      <c r="E474" s="2"/>
-      <c r="F474" s="2"/>
-      <c r="G474" s="2"/>
-      <c r="H474" s="2"/>
-      <c r="I474" s="2"/>
-      <c r="J474" s="2"/>
-      <c r="K474" s="2"/>
-      <c r="L474" s="2"/>
-      <c r="M474" s="2"/>
-      <c r="N474" s="2"/>
-      <c r="O474" s="2"/>
-      <c r="P474" s="2"/>
+      <c r="A474" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B474" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C474" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D474" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E474" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F474" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G474" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H474" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="I474" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J474" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="K474" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L474" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M474" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N474" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O474" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P474" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q474" s="2"/>
       <c r="R474" s="2"/>
       <c r="S474" s="2"/>
@@ -31021,22 +31743,48 @@
       <c r="Z474" s="2"/>
     </row>
     <row r="475" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A475" s="2"/>
-      <c r="B475" s="2"/>
-      <c r="C475" s="2"/>
-      <c r="D475" s="2"/>
-      <c r="E475" s="2"/>
-      <c r="F475" s="2"/>
-      <c r="G475" s="2"/>
-      <c r="H475" s="2"/>
-      <c r="I475" s="2"/>
-      <c r="J475" s="2"/>
-      <c r="K475" s="2"/>
-      <c r="L475" s="2"/>
-      <c r="M475" s="2"/>
-      <c r="N475" s="2"/>
-      <c r="O475" s="2"/>
-      <c r="P475" s="2"/>
+      <c r="A475" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="B475" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C475" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D475" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E475" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F475" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G475" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H475" s="6"/>
+      <c r="I475" s="6"/>
+      <c r="J475" s="6"/>
+      <c r="K475" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L475" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M475" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N475" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O475" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P475" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q475" s="2"/>
       <c r="R475" s="2"/>
       <c r="S475" s="2"/>
@@ -31049,22 +31797,52 @@
       <c r="Z475" s="2"/>
     </row>
     <row r="476" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A476" s="2"/>
-      <c r="B476" s="2"/>
-      <c r="C476" s="2"/>
-      <c r="D476" s="2"/>
-      <c r="E476" s="2"/>
-      <c r="F476" s="2"/>
-      <c r="G476" s="2"/>
-      <c r="H476" s="2"/>
-      <c r="I476" s="2"/>
-      <c r="J476" s="2"/>
-      <c r="K476" s="2"/>
-      <c r="L476" s="2"/>
-      <c r="M476" s="2"/>
-      <c r="N476" s="2"/>
-      <c r="O476" s="2"/>
-      <c r="P476" s="2"/>
+      <c r="A476" s="5" t="s">
+        <v>995</v>
+      </c>
+      <c r="B476" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C476" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D476" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E476" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F476" s="6"/>
+      <c r="G476" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H476" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="I476" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="J476" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="K476" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L476" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M476" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N476" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O476" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P476" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q476" s="2"/>
       <c r="R476" s="2"/>
       <c r="S476" s="2"/>
@@ -31077,22 +31855,54 @@
       <c r="Z476" s="2"/>
     </row>
     <row r="477" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A477" s="2"/>
-      <c r="B477" s="2"/>
-      <c r="C477" s="2"/>
-      <c r="D477" s="2"/>
-      <c r="E477" s="2"/>
-      <c r="F477" s="2"/>
-      <c r="G477" s="2"/>
-      <c r="H477" s="2"/>
-      <c r="I477" s="2"/>
-      <c r="J477" s="2"/>
-      <c r="K477" s="2"/>
-      <c r="L477" s="2"/>
-      <c r="M477" s="2"/>
-      <c r="N477" s="2"/>
-      <c r="O477" s="2"/>
-      <c r="P477" s="2"/>
+      <c r="A477" s="5" t="s">
+        <v>996</v>
+      </c>
+      <c r="B477" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C477" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D477" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E477" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F477" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G477" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H477" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="I477" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J477" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="K477" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L477" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M477" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N477" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O477" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P477" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q477" s="2"/>
       <c r="R477" s="2"/>
       <c r="S477" s="2"/>
@@ -31105,22 +31915,54 @@
       <c r="Z477" s="2"/>
     </row>
     <row r="478" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A478" s="2"/>
-      <c r="B478" s="2"/>
-      <c r="C478" s="2"/>
-      <c r="D478" s="2"/>
-      <c r="E478" s="2"/>
-      <c r="F478" s="2"/>
-      <c r="G478" s="2"/>
-      <c r="H478" s="2"/>
-      <c r="I478" s="2"/>
-      <c r="J478" s="2"/>
-      <c r="K478" s="2"/>
-      <c r="L478" s="2"/>
-      <c r="M478" s="2"/>
-      <c r="N478" s="2"/>
-      <c r="O478" s="2"/>
-      <c r="P478" s="2"/>
+      <c r="A478" s="5" t="s">
+        <v>997</v>
+      </c>
+      <c r="B478" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C478" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D478" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E478" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F478" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G478" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H478" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I478" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="J478" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="K478" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L478" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M478" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N478" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O478" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P478" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q478" s="2"/>
       <c r="R478" s="2"/>
       <c r="S478" s="2"/>
@@ -31133,22 +31975,54 @@
       <c r="Z478" s="2"/>
     </row>
     <row r="479" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A479" s="2"/>
-      <c r="B479" s="2"/>
-      <c r="C479" s="2"/>
-      <c r="D479" s="2"/>
-      <c r="E479" s="2"/>
-      <c r="F479" s="2"/>
-      <c r="G479" s="2"/>
-      <c r="H479" s="2"/>
-      <c r="I479" s="2"/>
-      <c r="J479" s="2"/>
-      <c r="K479" s="2"/>
-      <c r="L479" s="2"/>
-      <c r="M479" s="2"/>
-      <c r="N479" s="2"/>
-      <c r="O479" s="2"/>
-      <c r="P479" s="2"/>
+      <c r="A479" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B479" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C479" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D479" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E479" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F479" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G479" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H479" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I479" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="J479" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="K479" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L479" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M479" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N479" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O479" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P479" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q479" s="2"/>
       <c r="R479" s="2"/>
       <c r="S479" s="2"/>
@@ -31161,22 +32035,54 @@
       <c r="Z479" s="2"/>
     </row>
     <row r="480" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A480" s="2"/>
-      <c r="B480" s="2"/>
-      <c r="C480" s="2"/>
-      <c r="D480" s="2"/>
-      <c r="E480" s="2"/>
-      <c r="F480" s="2"/>
-      <c r="G480" s="2"/>
-      <c r="H480" s="2"/>
-      <c r="I480" s="2"/>
-      <c r="J480" s="2"/>
-      <c r="K480" s="2"/>
-      <c r="L480" s="2"/>
-      <c r="M480" s="2"/>
-      <c r="N480" s="2"/>
-      <c r="O480" s="2"/>
-      <c r="P480" s="2"/>
+      <c r="A480" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="B480" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C480" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D480" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E480" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F480" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G480" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H480" s="5" t="s">
+        <v>925</v>
+      </c>
+      <c r="I480" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J480" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="K480" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L480" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M480" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N480" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O480" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P480" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q480" s="2"/>
       <c r="R480" s="2"/>
       <c r="S480" s="2"/>
@@ -31189,22 +32095,48 @@
       <c r="Z480" s="2"/>
     </row>
     <row r="481" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A481" s="2"/>
-      <c r="B481" s="2"/>
-      <c r="C481" s="2"/>
-      <c r="D481" s="2"/>
-      <c r="E481" s="2"/>
-      <c r="F481" s="2"/>
-      <c r="G481" s="2"/>
-      <c r="H481" s="2"/>
-      <c r="I481" s="2"/>
-      <c r="J481" s="2"/>
-      <c r="K481" s="2"/>
-      <c r="L481" s="2"/>
-      <c r="M481" s="2"/>
-      <c r="N481" s="2"/>
-      <c r="O481" s="2"/>
-      <c r="P481" s="2"/>
+      <c r="A481" s="5" t="s">
+        <v>999</v>
+      </c>
+      <c r="B481" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C481" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D481" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E481" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F481" s="6"/>
+      <c r="G481" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H481" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="I481" s="6"/>
+      <c r="J481" s="6"/>
+      <c r="K481" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L481" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M481" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N481" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O481" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P481" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q481" s="2"/>
       <c r="R481" s="2"/>
       <c r="S481" s="2"/>
@@ -31217,22 +32149,54 @@
       <c r="Z481" s="2"/>
     </row>
     <row r="482" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A482" s="2"/>
-      <c r="B482" s="2"/>
-      <c r="C482" s="2"/>
-      <c r="D482" s="2"/>
-      <c r="E482" s="2"/>
-      <c r="F482" s="2"/>
-      <c r="G482" s="2"/>
-      <c r="H482" s="2"/>
-      <c r="I482" s="2"/>
-      <c r="J482" s="2"/>
-      <c r="K482" s="2"/>
-      <c r="L482" s="2"/>
-      <c r="M482" s="2"/>
-      <c r="N482" s="2"/>
-      <c r="O482" s="2"/>
-      <c r="P482" s="2"/>
+      <c r="A482" s="5" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B482" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C482" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D482" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E482" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F482" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G482" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H482" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="I482" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J482" s="5" t="s">
+        <v>1007</v>
+      </c>
+      <c r="K482" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L482" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M482" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N482" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O482" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P482" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q482" s="2"/>
       <c r="R482" s="2"/>
       <c r="S482" s="2"/>
@@ -31245,22 +32209,54 @@
       <c r="Z482" s="2"/>
     </row>
     <row r="483" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A483" s="2"/>
-      <c r="B483" s="2"/>
-      <c r="C483" s="2"/>
-      <c r="D483" s="2"/>
-      <c r="E483" s="2"/>
-      <c r="F483" s="2"/>
-      <c r="G483" s="2"/>
-      <c r="H483" s="2"/>
-      <c r="I483" s="2"/>
-      <c r="J483" s="2"/>
-      <c r="K483" s="2"/>
-      <c r="L483" s="2"/>
-      <c r="M483" s="2"/>
-      <c r="N483" s="2"/>
-      <c r="O483" s="2"/>
-      <c r="P483" s="2"/>
+      <c r="A483" s="5" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B483" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C483" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D483" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E483" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F483" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="G483" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H483" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I483" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="J483" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="K483" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L483" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M483" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N483" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O483" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P483" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q483" s="2"/>
       <c r="R483" s="2"/>
       <c r="S483" s="2"/>
@@ -31273,22 +32269,54 @@
       <c r="Z483" s="2"/>
     </row>
     <row r="484" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A484" s="2"/>
-      <c r="B484" s="2"/>
-      <c r="C484" s="2"/>
-      <c r="D484" s="2"/>
-      <c r="E484" s="2"/>
-      <c r="F484" s="2"/>
-      <c r="G484" s="2"/>
-      <c r="H484" s="2"/>
-      <c r="I484" s="2"/>
-      <c r="J484" s="2"/>
-      <c r="K484" s="2"/>
-      <c r="L484" s="2"/>
-      <c r="M484" s="2"/>
-      <c r="N484" s="2"/>
-      <c r="O484" s="2"/>
-      <c r="P484" s="2"/>
+      <c r="A484" s="5" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B484" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C484" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D484" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E484" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F484" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G484" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H484" s="5" t="s">
+        <v>1006</v>
+      </c>
+      <c r="I484" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="J484" s="5" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K484" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L484" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M484" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N484" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O484" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P484" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q484" s="2"/>
       <c r="R484" s="2"/>
       <c r="S484" s="2"/>
@@ -31301,22 +32329,54 @@
       <c r="Z484" s="2"/>
     </row>
     <row r="485" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A485" s="2"/>
-      <c r="B485" s="2"/>
-      <c r="C485" s="2"/>
-      <c r="D485" s="2"/>
-      <c r="E485" s="2"/>
-      <c r="F485" s="2"/>
-      <c r="G485" s="2"/>
-      <c r="H485" s="2"/>
-      <c r="I485" s="2"/>
-      <c r="J485" s="2"/>
-      <c r="K485" s="2"/>
-      <c r="L485" s="2"/>
-      <c r="M485" s="2"/>
-      <c r="N485" s="2"/>
-      <c r="O485" s="2"/>
-      <c r="P485" s="2"/>
+      <c r="A485" s="5" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B485" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C485" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D485" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E485" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F485" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G485" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H485" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I485" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="J485" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="K485" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L485" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M485" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N485" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O485" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P485" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q485" s="2"/>
       <c r="R485" s="2"/>
       <c r="S485" s="2"/>
@@ -31329,22 +32389,54 @@
       <c r="Z485" s="2"/>
     </row>
     <row r="486" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A486" s="2"/>
-      <c r="B486" s="2"/>
-      <c r="C486" s="2"/>
-      <c r="D486" s="2"/>
-      <c r="E486" s="2"/>
-      <c r="F486" s="2"/>
-      <c r="G486" s="2"/>
-      <c r="H486" s="2"/>
-      <c r="I486" s="2"/>
-      <c r="J486" s="2"/>
-      <c r="K486" s="2"/>
-      <c r="L486" s="2"/>
-      <c r="M486" s="2"/>
-      <c r="N486" s="2"/>
-      <c r="O486" s="2"/>
-      <c r="P486" s="2"/>
+      <c r="A486" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B486" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C486" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D486" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E486" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F486" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="G486" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H486" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="I486" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="J486" s="5" t="s">
+        <v>1010</v>
+      </c>
+      <c r="K486" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L486" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M486" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N486" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O486" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P486" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="Q486" s="2"/>
       <c r="R486" s="2"/>
       <c r="S486" s="2"/>
@@ -45665,7 +46757,7 @@
       <c r="Z997" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P428" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:P468" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>